<commit_message>
Merged PR 13120: Task Board Priorities + Sortability
Related work items: #97546
</commit_message>
<xml_diff>
--- a/AutomationTestingProgram/SampleTests/cser2.0.2.xlsx
+++ b/AutomationTestingProgram/SampleTests/cser2.0.2.xlsx
@@ -8,19 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ontariogov-my.sharepoint.com/personal/shaun_bautista_ontario_ca/Documents/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846C59A7-1BC4-4C64-9046-EAB64CA3C6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="13_ncr:1_{846C59A7-1BC4-4C64-9046-EAB64CA3C6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C33DDBB2-EE76-4C7A-AE01-3A4278083528}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CycleGroup1" sheetId="2" r:id="rId2"/>
+    <sheet name="Users" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="126">
   <si>
     <t>TESTCASENAME</t>
   </si>
@@ -91,9 +106,6 @@
     <t>MainContent_dlPFISCollection_hlpCollection_0</t>
   </si>
   <si>
-    <t>Select Algonquin College (ALGO)</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -145,9 +157,6 @@
     <t>Login</t>
   </si>
   <si>
-    <t>11150wasdA#</t>
-  </si>
-  <si>
     <t>Go to edcs9</t>
   </si>
   <si>
@@ -160,18 +169,6 @@
     <t>Shaun.Bautista@ontario.ca</t>
   </si>
   <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>{0}</t>
-  </si>
-  <si>
-    <t>{1}</t>
-  </si>
-  <si>
-    <t>{2}</t>
-  </si>
-  <si>
     <t>RunSQLScript</t>
   </si>
   <si>
@@ -286,12 +283,6 @@
     <t>cycleThree</t>
   </si>
   <si>
-    <t>[["C:/MyScripts/EDCS/CSER/sql_scripts/CSER_ReOpen_CAMB_Summer24-25.sql", "K:/ESIP/EDCS QA/QTP/CSER/Test Files/2024-25 Summer/2024-25 Summer CAMB 9708 (no errors).zip", "Cambrian College (CAMB)", "Summer Term 2024-25 (2024/06/30)"], ["C:/MyScripts/EDCS/CSER/sql_scripts/CSER_ReOpen_SSFL_Summer24-25.sql", "K:/ESIP/EDCS QA/QTP/CSER/Test Files/2024-25 Summer/2024-25 Summer SSFL 8826.zip", "Sir Sandford Fleming College (SSFL)", "Summer Term 2024-25 (2024/06/30)"]]</t>
-  </si>
-  <si>
-    <t>{3}</t>
-  </si>
-  <si>
     <t>2024-2025</t>
   </si>
   <si>
@@ -334,9 +325,6 @@
     <t>cmdSubmitFile</t>
   </si>
   <si>
-    <t>C:\Users\BautisSh\Downloads\Release Notes - EDCS 24.11.pdf</t>
-  </si>
-  <si>
     <t>Wait</t>
   </si>
   <si>
@@ -350,6 +338,81 @@
   </si>
   <si>
     <t>waitTwo</t>
+  </si>
+  <si>
+    <t>CYCLEGROUP</t>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>C:/MyScripts/EDCS/CSER/sql_scripts/CSER_ReOpen_CAMB_Summer24-25.sql</t>
+  </si>
+  <si>
+    <t>K:/ESIP/EDCS QA/QTP/CSER/Test Files/2024-25 Summer/2024-25 Summer CAMB 9708 (no errors).zip</t>
+  </si>
+  <si>
+    <t>Summer Term 2024-25 (2024/06/30)</t>
+  </si>
+  <si>
+    <t>CycleGroup1, START</t>
+  </si>
+  <si>
+    <t>CycleGroup1, END</t>
+  </si>
+  <si>
+    <t>SQLScript</t>
+  </si>
+  <si>
+    <t>DataFile</t>
+  </si>
+  <si>
+    <t>Submission</t>
+  </si>
+  <si>
+    <t>C:/MyScripts/EDCS/CSER/sql_scripts/CSER_ReOpen_SSFL_Summer24-25.sql</t>
+  </si>
+  <si>
+    <t>K:/ESIP/EDCS QA/QTP/CSER/Test Files/2024-25 Summer/2024-25 Summer SSFL 8826.zip</t>
+  </si>
+  <si>
+    <t>{SQLScript}</t>
+  </si>
+  <si>
+    <t>{Org}</t>
+  </si>
+  <si>
+    <t>{DataFile}</t>
+  </si>
+  <si>
+    <t>{Submission}</t>
+  </si>
+  <si>
+    <t>C:\Users\BautisSh\Downloads\password.txt</t>
+  </si>
+  <si>
+    <t>Email Address</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Role Codes</t>
+  </si>
+  <si>
+    <t>Org Codes</t>
+  </si>
+  <si>
+    <t>**********</t>
+  </si>
+  <si>
+    <t>Select Collège Boréal (SSFL)</t>
+  </si>
+  <si>
+    <t>Select Algonquin College (CAMB)</t>
+  </si>
+  <si>
+    <t>******</t>
   </si>
 </sst>
 </file>
@@ -419,14 +482,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -444,6 +506,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8AF61D59-9F93-49F5-91A5-F4718065E189}" name="Table1" displayName="Table1" ref="A1:O72" totalsRowShown="0">
+  <autoFilter ref="A1:O72" xr:uid="{8AF61D59-9F93-49F5-91A5-F4718065E189}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{29B1E5DD-2A54-491F-8314-51C90706DBC4}" name="TESTCASENAME"/>
+    <tableColumn id="2" xr3:uid="{97D0712C-9406-4535-A45E-8A46BA3AA10E}" name="TESTDESCRIPTION"/>
+    <tableColumn id="3" xr3:uid="{800DA51E-5D7B-41D1-9D1B-731E736A5E24}" name="STEPNUM"/>
+    <tableColumn id="4" xr3:uid="{2E0BA73F-C55A-453E-B5E8-44A8CA38F0F5}" name="ACTIONONOBJECT"/>
+    <tableColumn id="5" xr3:uid="{66D05A62-AAA9-4291-B9AB-45387F837CC2}" name="OBJECT"/>
+    <tableColumn id="6" xr3:uid="{43281A60-2B88-4291-9755-A0A88B2704C6}" name="VALUE"/>
+    <tableColumn id="7" xr3:uid="{619154CA-2EEB-4924-B7F9-8419A1D244F7}" name="COMMENTS"/>
+    <tableColumn id="8" xr3:uid="{3F273D6B-848F-4848-82B0-96E31F7BD0D6}" name="RELEASE"/>
+    <tableColumn id="9" xr3:uid="{42719DD0-F5FE-4733-8AEA-DDF60C0FFDA9}" name="LOCAL_ATTEMPTS"/>
+    <tableColumn id="10" xr3:uid="{EF0CD3E0-066E-4755-B0FE-4E97564BC8D1}" name="LOCAL_TIMEOUT"/>
+    <tableColumn id="11" xr3:uid="{5AF0F111-AC8C-4D81-BCDD-D56CED388CF7}" name="CONTROL"/>
+    <tableColumn id="12" xr3:uid="{B705B4EC-8B02-453E-9916-B610B35C9848}" name="COLLECTION"/>
+    <tableColumn id="13" xr3:uid="{365464DC-C8DA-409A-AD99-A126599D6C05}" name="TESTSTEPTYPE"/>
+    <tableColumn id="14" xr3:uid="{04745E9C-14B7-484B-A3BB-4AC4D5AC2BA9}" name="GOTOSTEP"/>
+    <tableColumn id="15" xr3:uid="{190B6F41-6431-4B31-B658-AA6ED03584D6}" name="CYCLEGROUP"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -768,28 +854,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O78"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.375" customWidth="1"/>
-    <col min="6" max="6" width="80" customWidth="1"/>
-    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="221.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="71.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -836,7 +923,7 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -844,16 +931,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -861,19 +948,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>41</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -966,22 +1053,22 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>113</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
         <v>18</v>
@@ -1005,31 +1092,31 @@
         <v>18</v>
       </c>
       <c r="O6" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" t="s">
-        <v>27</v>
-      </c>
       <c r="H7" t="s">
         <v>18</v>
       </c>
@@ -1050,32 +1137,29 @@
       </c>
       <c r="N7" t="s">
         <v>18</v>
-      </c>
-      <c r="O7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" t="s">
         <v>18</v>
@@ -1101,20 +1185,20 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
       <c r="F9" t="s">
         <v>18</v>
       </c>
@@ -1141,32 +1225,29 @@
       </c>
       <c r="N9" t="s">
         <v>18</v>
-      </c>
-      <c r="O9" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" t="s">
         <v>18</v>
@@ -1188,27 +1269,24 @@
       </c>
       <c r="N10" t="s">
         <v>18</v>
-      </c>
-      <c r="O10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="D11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
       <c r="F11" t="s">
         <v>18</v>
       </c>
@@ -1235,26 +1313,23 @@
       </c>
       <c r="N11" t="s">
         <v>18</v>
-      </c>
-      <c r="O11" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>18</v>
@@ -1282,32 +1357,29 @@
       </c>
       <c r="N12" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>48</v>
+        <v>115</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>18</v>
@@ -1329,26 +1401,23 @@
       </c>
       <c r="N13" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O13" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>18</v>
@@ -1376,26 +1445,23 @@
       </c>
       <c r="N14" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O14" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>18</v>
@@ -1424,50 +1490,49 @@
       <c r="N15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O15" t="s">
-        <v>88</v>
+      <c r="O15" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C16" s="4">
         <v>1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F16" s="4">
-        <v>180</v>
-      </c>
-      <c r="O16" s="3"/>
-    </row>
-    <row r="17" spans="1:15" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="F17" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="H17" s="5" t="s">
         <v>18</v>
       </c>
@@ -1486,31 +1551,31 @@
       <c r="N17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O17" s="6" t="s">
-        <v>88</v>
+      <c r="O17" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>18</v>
@@ -1532,26 +1597,23 @@
       </c>
       <c r="N18" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O18" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>18</v>
@@ -1579,32 +1641,29 @@
       </c>
       <c r="N19" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O19" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>18</v>
@@ -1626,26 +1685,23 @@
       </c>
       <c r="N20" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O20" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>18</v>
@@ -1673,26 +1729,23 @@
       </c>
       <c r="N21" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O21" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>18</v>
@@ -1720,26 +1773,23 @@
       </c>
       <c r="N22" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O22" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:15" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>18</v>
@@ -1764,26 +1814,23 @@
       </c>
       <c r="N23" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="O23" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>18</v>
@@ -1811,26 +1858,23 @@
       </c>
       <c r="N24" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O24" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>18</v>
@@ -1859,50 +1903,49 @@
       <c r="N25" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O25" t="s">
-        <v>88</v>
+      <c r="O25" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C26" s="4">
         <v>1</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F26" s="4">
-        <v>240</v>
-      </c>
-      <c r="O26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="F27" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="H27" s="5" t="s">
         <v>18</v>
       </c>
@@ -1921,31 +1964,31 @@
       <c r="N27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="O27" s="6" t="s">
-        <v>88</v>
+      <c r="O27" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>18</v>
@@ -1967,26 +2010,23 @@
       </c>
       <c r="N28" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O28" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>18</v>
@@ -2014,32 +2054,29 @@
       </c>
       <c r="N29" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O29" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>18</v>
@@ -2061,26 +2098,23 @@
       </c>
       <c r="N30" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O30" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>18</v>
@@ -2108,26 +2142,23 @@
       </c>
       <c r="N31" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O31" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>18</v>
@@ -2155,26 +2186,23 @@
       </c>
       <c r="N32" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O32" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>19</v>
@@ -2196,26 +2224,23 @@
       </c>
       <c r="N33" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="O33" s="6" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>18</v>
@@ -2240,26 +2265,23 @@
       </c>
       <c r="N34" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O34" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>18</v>
@@ -2287,63 +2309,60 @@
       </c>
       <c r="N35" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O35" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O36" t="s">
-        <v>88</v>
+        <v>76</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>18</v>
@@ -2368,14 +2387,11 @@
       </c>
       <c r="N38" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O38" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
@@ -2416,13 +2432,10 @@
       <c r="N39" t="s">
         <v>18</v>
       </c>
-      <c r="O39" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
         <v>20</v>
@@ -2463,32 +2476,29 @@
       <c r="N40" t="s">
         <v>18</v>
       </c>
-      <c r="O40" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="41" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F41" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="H41" s="2" t="s">
         <v>18</v>
       </c>
@@ -2511,30 +2521,30 @@
         <v>18</v>
       </c>
       <c r="O41" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>18</v>
@@ -2556,26 +2566,23 @@
       </c>
       <c r="N42" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O42" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>18</v>
@@ -2603,32 +2610,29 @@
       </c>
       <c r="N43" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O43" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="44" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>18</v>
@@ -2650,26 +2654,23 @@
       </c>
       <c r="N44" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O44" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>18</v>
@@ -2697,26 +2698,23 @@
       </c>
       <c r="N45" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O45" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>18</v>
@@ -2744,26 +2742,23 @@
       </c>
       <c r="N46" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O46" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>18</v>
@@ -2791,26 +2786,23 @@
       </c>
       <c r="N47" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O47" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>18</v>
@@ -2838,26 +2830,23 @@
       </c>
       <c r="N48" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O48" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>18</v>
@@ -2886,50 +2875,50 @@
       <c r="N49" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O49" t="s">
-        <v>88</v>
+      <c r="O49" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C50">
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C51">
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
         <v>15</v>
@@ -2971,12 +2960,12 @@
         <v>18</v>
       </c>
       <c r="O52" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B53" t="s">
         <v>20</v>
@@ -3017,32 +3006,29 @@
       <c r="N53" t="s">
         <v>18</v>
       </c>
-      <c r="O53" t="s">
-        <v>88</v>
-      </c>
     </row>
     <row r="54" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D54" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G54" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F54" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="H54" s="2" t="s">
         <v>18</v>
       </c>
@@ -3060,32 +3046,29 @@
       </c>
       <c r="N54" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O54" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>18</v>
@@ -3107,26 +3090,23 @@
       </c>
       <c r="N55" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O55" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>18</v>
@@ -3154,32 +3134,29 @@
       </c>
       <c r="N56" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O56" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H57" s="2" t="s">
         <v>18</v>
@@ -3201,26 +3178,23 @@
       </c>
       <c r="N57" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O57" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D58" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>18</v>
@@ -3248,26 +3222,23 @@
       </c>
       <c r="N58" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O58" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="59" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>18</v>
@@ -3295,26 +3266,23 @@
       </c>
       <c r="N59" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O59" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="60" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>18</v>
@@ -3342,26 +3310,23 @@
       </c>
       <c r="N60" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O60" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="61" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>18</v>
@@ -3389,26 +3354,23 @@
       </c>
       <c r="N61" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O61" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="62" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D62" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>18</v>
@@ -3436,33 +3398,30 @@
       </c>
       <c r="N62" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O62" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="63" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D63" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="H63" s="2" t="s">
         <v>18</v>
       </c>
@@ -3483,32 +3442,29 @@
       </c>
       <c r="N63" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O63" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="64" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>18</v>
@@ -3530,26 +3486,23 @@
       </c>
       <c r="N64" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O64" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D65" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>18</v>
@@ -3577,32 +3530,29 @@
       </c>
       <c r="N65" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O65" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="66" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H66" s="2" t="s">
         <v>18</v>
@@ -3624,26 +3574,23 @@
       </c>
       <c r="N66" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O66" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="67" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>18</v>
@@ -3671,26 +3618,23 @@
       </c>
       <c r="N67" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O67" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="68" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>18</v>
@@ -3718,26 +3662,23 @@
       </c>
       <c r="N68" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O68" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="69" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D69" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>18</v>
@@ -3765,32 +3706,29 @@
       </c>
       <c r="N69" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O69" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H70" s="2" t="s">
         <v>18</v>
@@ -3812,26 +3750,23 @@
       </c>
       <c r="N70" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O70" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="71" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>18</v>
@@ -3859,26 +3794,23 @@
       </c>
       <c r="N71" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="O71" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="72" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>16</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>18</v>
@@ -3907,38 +3839,8 @@
       <c r="N72" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O72" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O73" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O74" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O75" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O76" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O77" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O78" t="s">
-        <v>88</v>
+      <c r="O72" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3949,9 +3851,114 @@
     <hyperlink ref="E51" r:id="rId3" xr:uid="{5C15914A-A4E4-4F8D-9E6E-8D11E80A81BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B5:N5 A1:N1 B9:N9 B7:E7 G7:N7 B8:E8 G8:N8 B11:N11 B10:E10 G10:N10 B4:N4" numberStoredAsText="1"/>
-  </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD8A481E-4312-4BB7-973A-96CD3C5B6711}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.375" customWidth="1"/>
+    <col min="6" max="6" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="84.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D117A5-151D-4035-8B1C-FD2138E0073E}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>